<commit_message>
Added Catskill, file organization
</commit_message>
<xml_diff>
--- a/Output/Census/County_Census.xlsx
+++ b/Output/Census/County_Census.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26327"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://esf0-my.sharepoint.com/personal/jmelliot_esf_edu/Documents/Summer 23/754 MPA Workshop/Adirontax Github/Tax Rates &amp; Parcels/Output/Census/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="11_89395FB1D21782116D2C4C0C352C31137878ABA5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8F181ABE-9875-4429-9E8C-35A607E24746}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="1070" yWindow="1340" windowWidth="24930" windowHeight="13390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="County_Census" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -805,8 +799,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -869,14 +863,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -923,7 +909,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -955,27 +941,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1007,24 +975,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1200,30 +1150,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="2.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.08984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.08984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.54296875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.6328125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.453125" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1258,7 +1192,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1296,7 +1230,7 @@
         <v>2129</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1334,7 +1268,7 @@
         <v>6490</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1372,7 +1306,7 @@
         <v>10611</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1392,7 +1326,7 @@
         <v>76</v>
       </c>
       <c r="G5">
-        <v>36.930999999999997</v>
+        <v>36.931</v>
       </c>
       <c r="H5">
         <v>1693702.3</v>
@@ -1410,7 +1344,7 @@
         <v>7065</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1433,7 +1367,7 @@
         <v>40.96</v>
       </c>
       <c r="H6">
-        <v>9468486.4000000004</v>
+        <v>9468486.4</v>
       </c>
       <c r="I6" t="s">
         <v>202</v>
@@ -1448,7 +1382,7 @@
         <v>67981</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1468,7 +1402,7 @@
         <v>78</v>
       </c>
       <c r="G7">
-        <v>32.764000000000003</v>
+        <v>32.764</v>
       </c>
       <c r="H7">
         <v>849234.9</v>
@@ -1486,7 +1420,7 @@
         <v>2622</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1506,7 +1440,7 @@
         <v>79</v>
       </c>
       <c r="G8">
-        <v>35.200000000000003</v>
+        <v>35.2</v>
       </c>
       <c r="H8">
         <v>1359235.3</v>
@@ -1524,7 +1458,7 @@
         <v>4904</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1544,10 +1478,10 @@
         <v>80</v>
       </c>
       <c r="G9">
-        <v>34.511000000000003</v>
+        <v>34.511</v>
       </c>
       <c r="H9">
-        <v>1315745.8999999999</v>
+        <v>1315745.9</v>
       </c>
       <c r="I9" t="s">
         <v>205</v>
@@ -1562,7 +1496,7 @@
         <v>3220</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1582,7 +1516,7 @@
         <v>81</v>
       </c>
       <c r="G10">
-        <v>33.262999999999998</v>
+        <v>33.263</v>
       </c>
       <c r="H10">
         <v>541872.5</v>
@@ -1600,7 +1534,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1620,10 +1554,10 @@
         <v>82</v>
       </c>
       <c r="G11">
-        <v>36.399000000000001</v>
+        <v>36.399</v>
       </c>
       <c r="H11">
-        <v>20169327.399999999</v>
+        <v>20169327.4</v>
       </c>
       <c r="I11" t="s">
         <v>207</v>
@@ -1638,7 +1572,7 @@
         <v>188167</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1658,10 +1592,10 @@
         <v>83</v>
       </c>
       <c r="G12">
-        <v>63.417999999999999</v>
+        <v>63.418</v>
       </c>
       <c r="H12">
-        <v>108675922.90000001</v>
+        <v>108675922.9</v>
       </c>
       <c r="I12" t="s">
         <v>208</v>
@@ -1676,7 +1610,7 @@
         <v>730430</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1696,10 +1630,10 @@
         <v>84</v>
       </c>
       <c r="G13">
-        <v>37.866999999999997</v>
+        <v>37.867</v>
       </c>
       <c r="H13">
-        <v>12395152.199999999</v>
+        <v>12395152.2</v>
       </c>
       <c r="I13" t="s">
         <v>209</v>
@@ -1714,7 +1648,7 @@
         <v>97922</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1734,7 +1668,7 @@
         <v>85</v>
       </c>
       <c r="G14">
-        <v>31.954999999999998</v>
+        <v>31.955</v>
       </c>
       <c r="H14">
         <v>777659.5</v>
@@ -1752,7 +1686,7 @@
         <v>4711</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1790,7 +1724,7 @@
         <v>14766</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1810,7 +1744,7 @@
         <v>87</v>
       </c>
       <c r="G16">
-        <v>48.341999999999999</v>
+        <v>48.342</v>
       </c>
       <c r="H16">
         <v>14528103.6</v>
@@ -1828,7 +1762,7 @@
         <v>135160</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1848,10 +1782,10 @@
         <v>88</v>
       </c>
       <c r="G17">
-        <v>39.232999999999997</v>
+        <v>39.233</v>
       </c>
       <c r="H17">
-        <v>9141055.6999999993</v>
+        <v>9141055.699999999</v>
       </c>
       <c r="I17" t="s">
         <v>213</v>
@@ -1866,7 +1800,7 @@
         <v>79087</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1886,10 +1820,10 @@
         <v>89</v>
       </c>
       <c r="G18">
-        <v>30.173999999999999</v>
+        <v>30.174</v>
       </c>
       <c r="H18">
-        <v>26567691.699999999</v>
+        <v>26567691.7</v>
       </c>
       <c r="I18" t="s">
         <v>214</v>
@@ -1904,7 +1838,7 @@
         <v>1120487</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1924,7 +1858,7 @@
         <v>90</v>
       </c>
       <c r="G19">
-        <v>30.617999999999999</v>
+        <v>30.618</v>
       </c>
       <c r="H19">
         <v>4129329.4</v>
@@ -1942,7 +1876,7 @@
         <v>29489</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -1962,7 +1896,7 @@
         <v>91</v>
       </c>
       <c r="G20">
-        <v>35.119999999999997</v>
+        <v>35.12</v>
       </c>
       <c r="H20">
         <v>1770555.4</v>
@@ -1980,7 +1914,7 @@
         <v>6910</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:12">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -2018,7 +1952,7 @@
         <v>11538</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:12">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -2038,7 +1972,7 @@
         <v>93</v>
       </c>
       <c r="G22">
-        <v>32.405000000000001</v>
+        <v>32.405</v>
       </c>
       <c r="H22">
         <v>972042.3</v>
@@ -2056,7 +1990,7 @@
         <v>2065</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:12">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -2076,7 +2010,7 @@
         <v>94</v>
       </c>
       <c r="G23">
-        <v>33.957000000000001</v>
+        <v>33.957</v>
       </c>
       <c r="H23">
         <v>1740879.6</v>
@@ -2094,7 +2028,7 @@
         <v>7685</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:12">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -2114,10 +2048,10 @@
         <v>95</v>
       </c>
       <c r="G24">
-        <v>30.234000000000002</v>
+        <v>30.234</v>
       </c>
       <c r="H24">
-        <v>1050944.3999999999</v>
+        <v>1050944.4</v>
       </c>
       <c r="I24" t="s">
         <v>220</v>
@@ -2132,7 +2066,7 @@
         <v>2903</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:12">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -2152,7 +2086,7 @@
         <v>96</v>
       </c>
       <c r="G25">
-        <v>29.388999999999999</v>
+        <v>29.389</v>
       </c>
       <c r="H25">
         <v>838351</v>
@@ -2170,7 +2104,7 @@
         <v>2802</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:12">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -2190,7 +2124,7 @@
         <v>97</v>
       </c>
       <c r="G26">
-        <v>37.551000000000002</v>
+        <v>37.551</v>
       </c>
       <c r="H26">
         <v>24689589.5</v>
@@ -2208,7 +2142,7 @@
         <v>210522</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:12">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -2228,7 +2162,7 @@
         <v>98</v>
       </c>
       <c r="G27">
-        <v>33.027999999999999</v>
+        <v>33.028</v>
       </c>
       <c r="H27">
         <v>958643.5</v>
@@ -2246,7 +2180,7 @@
         <v>8937</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:12">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -2266,7 +2200,7 @@
         <v>99</v>
       </c>
       <c r="G28">
-        <v>32.853999999999999</v>
+        <v>32.854</v>
       </c>
       <c r="H28">
         <v>1184315.3</v>
@@ -2284,7 +2218,7 @@
         <v>3756</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:12">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -2304,7 +2238,7 @@
         <v>100</v>
       </c>
       <c r="G29">
-        <v>35.276000000000003</v>
+        <v>35.276</v>
       </c>
       <c r="H29">
         <v>1036525.5</v>
@@ -2322,7 +2256,7 @@
         <v>5464</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:12">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -2342,10 +2276,10 @@
         <v>101</v>
       </c>
       <c r="G30">
-        <v>31.603000000000002</v>
+        <v>31.603</v>
       </c>
       <c r="H30">
-        <v>82826.600000000006</v>
+        <v>82826.60000000001</v>
       </c>
       <c r="I30" t="s">
         <v>226</v>
@@ -2360,7 +2294,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:12">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -2383,7 +2317,7 @@
         <v>31.134</v>
       </c>
       <c r="H31">
-        <v>2399187.2000000002</v>
+        <v>2399187.2</v>
       </c>
       <c r="I31" t="s">
         <v>227</v>
@@ -2398,7 +2332,7 @@
         <v>16160</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:12">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -2418,10 +2352,10 @@
         <v>103</v>
       </c>
       <c r="G32">
-        <v>41.558999999999997</v>
+        <v>41.559</v>
       </c>
       <c r="H32">
-        <v>80257344.200000003</v>
+        <v>80257344.2</v>
       </c>
       <c r="I32" t="s">
         <v>228</v>
@@ -2436,7 +2370,7 @@
         <v>1473566</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:12">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -2474,7 +2408,7 @@
         <v>5091</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:12">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -2512,7 +2446,7 @@
         <v>4629</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:12">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -2532,7 +2466,7 @@
         <v>106</v>
       </c>
       <c r="G35">
-        <v>32.298999999999999</v>
+        <v>32.299</v>
       </c>
       <c r="H35">
         <v>1025777.2</v>
@@ -2550,7 +2484,7 @@
         <v>6669</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:12">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -2573,7 +2507,7 @@
         <v>52.814</v>
       </c>
       <c r="H36">
-        <v>58936669.299999997</v>
+        <v>58936669.3</v>
       </c>
       <c r="I36" t="s">
         <v>232</v>
@@ -2588,7 +2522,7 @@
         <v>456761</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:12">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -2626,7 +2560,7 @@
         <v>28346</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:12">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -2646,10 +2580,10 @@
         <v>109</v>
       </c>
       <c r="G38">
-        <v>35.293999999999997</v>
+        <v>35.294</v>
       </c>
       <c r="H38">
-        <v>5128666.5999999996</v>
+        <v>5128666.6</v>
       </c>
       <c r="I38" t="s">
         <v>234</v>
@@ -2664,7 +2598,7 @@
         <v>35614</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:12">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -2684,7 +2618,7 @@
         <v>110</v>
       </c>
       <c r="G39">
-        <v>35.905999999999999</v>
+        <v>35.906</v>
       </c>
       <c r="H39">
         <v>3069865.5</v>
@@ -2702,7 +2636,7 @@
         <v>8810</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:12">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -2740,7 +2674,7 @@
         <v>104956</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:12">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -2760,10 +2694,10 @@
         <v>112</v>
       </c>
       <c r="G41">
-        <v>31.818000000000001</v>
+        <v>31.818</v>
       </c>
       <c r="H41">
-        <v>2610294.2000000002</v>
+        <v>2610294.2</v>
       </c>
       <c r="I41" t="s">
         <v>237</v>
@@ -2778,7 +2712,7 @@
         <v>6028</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:12">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -2798,10 +2732,10 @@
         <v>113</v>
       </c>
       <c r="G42">
-        <v>28.172999999999998</v>
+        <v>28.173</v>
       </c>
       <c r="H42">
-        <v>1302227.1000000001</v>
+        <v>1302227.1</v>
       </c>
       <c r="I42" t="s">
         <v>238</v>
@@ -2816,7 +2750,7 @@
         <v>4270</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:12">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -2836,10 +2770,10 @@
         <v>114</v>
       </c>
       <c r="G43">
-        <v>39.755000000000003</v>
+        <v>39.755</v>
       </c>
       <c r="H43">
-        <v>63935238.700000003</v>
+        <v>63935238.7</v>
       </c>
       <c r="I43" t="s">
         <v>239</v>
@@ -2854,7 +2788,7 @@
         <v>1456623</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:12">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -2874,7 +2808,7 @@
         <v>115</v>
       </c>
       <c r="G44">
-        <v>41.646999999999998</v>
+        <v>41.647</v>
       </c>
       <c r="H44">
         <v>4565659.7</v>
@@ -2892,7 +2826,7 @@
         <v>23912</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:12">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -2912,10 +2846,10 @@
         <v>116</v>
       </c>
       <c r="G45">
-        <v>42.697000000000003</v>
+        <v>42.697</v>
       </c>
       <c r="H45">
-        <v>10395197.300000001</v>
+        <v>10395197.3</v>
       </c>
       <c r="I45" t="s">
         <v>241</v>
@@ -2930,7 +2864,7 @@
         <v>97740</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:12">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -2950,7 +2884,7 @@
         <v>117</v>
       </c>
       <c r="G46">
-        <v>30.882000000000001</v>
+        <v>30.882</v>
       </c>
       <c r="H46">
         <v>2075579.4</v>
@@ -2968,7 +2902,7 @@
         <v>8044</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:12">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -2991,7 +2925,7 @@
         <v>46.71</v>
       </c>
       <c r="H47">
-        <v>8346047.4000000004</v>
+        <v>8346047.4</v>
       </c>
       <c r="I47" t="s">
         <v>243</v>
@@ -3006,7 +2940,7 @@
         <v>18055</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:12">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -3026,7 +2960,7 @@
         <v>119</v>
       </c>
       <c r="G48">
-        <v>37.356000000000002</v>
+        <v>37.356</v>
       </c>
       <c r="H48">
         <v>3892732.7</v>
@@ -3044,7 +2978,7 @@
         <v>38095</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:12">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -3064,7 +2998,7 @@
         <v>120</v>
       </c>
       <c r="G49">
-        <v>33.563000000000002</v>
+        <v>33.563</v>
       </c>
       <c r="H49">
         <v>733691.9</v>
@@ -3082,7 +3016,7 @@
         <v>1918</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:12">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -3102,7 +3036,7 @@
         <v>121</v>
       </c>
       <c r="G50">
-        <v>32.113999999999997</v>
+        <v>32.114</v>
       </c>
       <c r="H50">
         <v>377443.2</v>
@@ -3120,7 +3054,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:12">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -3140,7 +3074,7 @@
         <v>122</v>
       </c>
       <c r="G51">
-        <v>31.998000000000001</v>
+        <v>31.998</v>
       </c>
       <c r="H51">
         <v>693479.4</v>
@@ -3158,7 +3092,7 @@
         <v>3291</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:12">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -3196,7 +3130,7 @@
         <v>5739</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:12">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -3219,7 +3153,7 @@
         <v>48.177</v>
       </c>
       <c r="H53">
-        <v>55140618.600000001</v>
+        <v>55140618.6</v>
       </c>
       <c r="I53" t="s">
         <v>249</v>
@@ -3234,7 +3168,7 @@
         <v>319503</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:12">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -3254,7 +3188,7 @@
         <v>125</v>
       </c>
       <c r="G54">
-        <v>35.798000000000002</v>
+        <v>35.798</v>
       </c>
       <c r="H54">
         <v>1794190.4</v>
@@ -3272,7 +3206,7 @@
         <v>16343</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:12">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -3292,7 +3226,7 @@
         <v>126</v>
       </c>
       <c r="G55">
-        <v>35.192999999999998</v>
+        <v>35.193</v>
       </c>
       <c r="H55">
         <v>1171454.7</v>
@@ -3310,7 +3244,7 @@
         <v>2045</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:12">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -3330,7 +3264,7 @@
         <v>127</v>
       </c>
       <c r="G56">
-        <v>29.774000000000001</v>
+        <v>29.774</v>
       </c>
       <c r="H56">
         <v>2701530.3</v>
@@ -3348,7 +3282,7 @@
         <v>20869</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:12">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -3371,7 +3305,7 @@
         <v>36.244</v>
       </c>
       <c r="H57">
-        <v>4810770.9000000004</v>
+        <v>4810770.9</v>
       </c>
       <c r="I57" t="s">
         <v>253</v>
@@ -3386,7 +3320,7 @@
         <v>32308</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:12">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -3406,7 +3340,7 @@
         <v>129</v>
       </c>
       <c r="G58">
-        <v>38.118000000000002</v>
+        <v>38.118</v>
       </c>
       <c r="H58">
         <v>1827294.9</v>
@@ -3424,7 +3358,7 @@
         <v>2892</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:12">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -3444,10 +3378,10 @@
         <v>130</v>
       </c>
       <c r="G59">
-        <v>34.706000000000003</v>
+        <v>34.706</v>
       </c>
       <c r="H59">
-        <v>1285477.3999999999</v>
+        <v>1285477.4</v>
       </c>
       <c r="I59" t="s">
         <v>255</v>
@@ -3462,7 +3396,7 @@
         <v>4531</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:12">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -3482,10 +3416,10 @@
         <v>131</v>
       </c>
       <c r="G60">
-        <v>34.460999999999999</v>
+        <v>34.461</v>
       </c>
       <c r="H60">
-        <v>2153154.2000000002</v>
+        <v>2153154.2</v>
       </c>
       <c r="I60" t="s">
         <v>256</v>
@@ -3500,7 +3434,7 @@
         <v>7504</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:12">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -3520,10 +3454,10 @@
         <v>132</v>
       </c>
       <c r="G61">
-        <v>50.561999999999998</v>
+        <v>50.562</v>
       </c>
       <c r="H61">
-        <v>46222976.200000003</v>
+        <v>46222976.2</v>
       </c>
       <c r="I61" t="s">
         <v>257</v>
@@ -3538,7 +3472,7 @@
         <v>370351</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:12">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -3558,7 +3492,7 @@
         <v>133</v>
       </c>
       <c r="G62">
-        <v>35.082000000000001</v>
+        <v>35.082</v>
       </c>
       <c r="H62">
         <v>893158.6</v>
@@ -3576,7 +3510,7 @@
         <v>3548</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:12">
       <c r="A63" s="1">
         <v>61</v>
       </c>

</xml_diff>

<commit_message>
Re-sync from onedrive issue
</commit_message>
<xml_diff>
--- a/Output/Census/County_Census.xlsx
+++ b/Output/Census/County_Census.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26327"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://esf0-my.sharepoint.com/personal/jmelliot_esf_edu/Documents/Summer 23/754 MPA Workshop/Adirontax Github/Tax Rates &amp; Parcels/Output/Census/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="11_89395FB1D21782116D2C4C0C352C31137878ABA5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8F181ABE-9875-4429-9E8C-35A607E24746}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="1070" yWindow="1340" windowWidth="24930" windowHeight="13390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="County_Census" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -805,8 +799,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -869,14 +863,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -923,7 +909,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -955,27 +941,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1007,24 +975,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1200,30 +1150,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="2.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.08984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.08984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.54296875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.6328125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.453125" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1258,7 +1192,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1296,7 +1230,7 @@
         <v>2129</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1334,7 +1268,7 @@
         <v>6490</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1372,7 +1306,7 @@
         <v>10611</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1392,7 +1326,7 @@
         <v>76</v>
       </c>
       <c r="G5">
-        <v>36.930999999999997</v>
+        <v>36.931</v>
       </c>
       <c r="H5">
         <v>1693702.3</v>
@@ -1410,7 +1344,7 @@
         <v>7065</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1433,7 +1367,7 @@
         <v>40.96</v>
       </c>
       <c r="H6">
-        <v>9468486.4000000004</v>
+        <v>9468486.4</v>
       </c>
       <c r="I6" t="s">
         <v>202</v>
@@ -1448,7 +1382,7 @@
         <v>67981</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1468,7 +1402,7 @@
         <v>78</v>
       </c>
       <c r="G7">
-        <v>32.764000000000003</v>
+        <v>32.764</v>
       </c>
       <c r="H7">
         <v>849234.9</v>
@@ -1486,7 +1420,7 @@
         <v>2622</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1506,7 +1440,7 @@
         <v>79</v>
       </c>
       <c r="G8">
-        <v>35.200000000000003</v>
+        <v>35.2</v>
       </c>
       <c r="H8">
         <v>1359235.3</v>
@@ -1524,7 +1458,7 @@
         <v>4904</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1544,10 +1478,10 @@
         <v>80</v>
       </c>
       <c r="G9">
-        <v>34.511000000000003</v>
+        <v>34.511</v>
       </c>
       <c r="H9">
-        <v>1315745.8999999999</v>
+        <v>1315745.9</v>
       </c>
       <c r="I9" t="s">
         <v>205</v>
@@ -1562,7 +1496,7 @@
         <v>3220</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1582,7 +1516,7 @@
         <v>81</v>
       </c>
       <c r="G10">
-        <v>33.262999999999998</v>
+        <v>33.263</v>
       </c>
       <c r="H10">
         <v>541872.5</v>
@@ -1600,7 +1534,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1620,10 +1554,10 @@
         <v>82</v>
       </c>
       <c r="G11">
-        <v>36.399000000000001</v>
+        <v>36.399</v>
       </c>
       <c r="H11">
-        <v>20169327.399999999</v>
+        <v>20169327.4</v>
       </c>
       <c r="I11" t="s">
         <v>207</v>
@@ -1638,7 +1572,7 @@
         <v>188167</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1658,10 +1592,10 @@
         <v>83</v>
       </c>
       <c r="G12">
-        <v>63.417999999999999</v>
+        <v>63.418</v>
       </c>
       <c r="H12">
-        <v>108675922.90000001</v>
+        <v>108675922.9</v>
       </c>
       <c r="I12" t="s">
         <v>208</v>
@@ -1676,7 +1610,7 @@
         <v>730430</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1696,10 +1630,10 @@
         <v>84</v>
       </c>
       <c r="G13">
-        <v>37.866999999999997</v>
+        <v>37.867</v>
       </c>
       <c r="H13">
-        <v>12395152.199999999</v>
+        <v>12395152.2</v>
       </c>
       <c r="I13" t="s">
         <v>209</v>
@@ -1714,7 +1648,7 @@
         <v>97922</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1734,7 +1668,7 @@
         <v>85</v>
       </c>
       <c r="G14">
-        <v>31.954999999999998</v>
+        <v>31.955</v>
       </c>
       <c r="H14">
         <v>777659.5</v>
@@ -1752,7 +1686,7 @@
         <v>4711</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1790,7 +1724,7 @@
         <v>14766</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1810,7 +1744,7 @@
         <v>87</v>
       </c>
       <c r="G16">
-        <v>48.341999999999999</v>
+        <v>48.342</v>
       </c>
       <c r="H16">
         <v>14528103.6</v>
@@ -1828,7 +1762,7 @@
         <v>135160</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1848,10 +1782,10 @@
         <v>88</v>
       </c>
       <c r="G17">
-        <v>39.232999999999997</v>
+        <v>39.233</v>
       </c>
       <c r="H17">
-        <v>9141055.6999999993</v>
+        <v>9141055.699999999</v>
       </c>
       <c r="I17" t="s">
         <v>213</v>
@@ -1866,7 +1800,7 @@
         <v>79087</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1886,10 +1820,10 @@
         <v>89</v>
       </c>
       <c r="G18">
-        <v>30.173999999999999</v>
+        <v>30.174</v>
       </c>
       <c r="H18">
-        <v>26567691.699999999</v>
+        <v>26567691.7</v>
       </c>
       <c r="I18" t="s">
         <v>214</v>
@@ -1904,7 +1838,7 @@
         <v>1120487</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1924,7 +1858,7 @@
         <v>90</v>
       </c>
       <c r="G19">
-        <v>30.617999999999999</v>
+        <v>30.618</v>
       </c>
       <c r="H19">
         <v>4129329.4</v>
@@ -1942,7 +1876,7 @@
         <v>29489</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -1962,7 +1896,7 @@
         <v>91</v>
       </c>
       <c r="G20">
-        <v>35.119999999999997</v>
+        <v>35.12</v>
       </c>
       <c r="H20">
         <v>1770555.4</v>
@@ -1980,7 +1914,7 @@
         <v>6910</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:12">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -2018,7 +1952,7 @@
         <v>11538</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:12">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -2038,7 +1972,7 @@
         <v>93</v>
       </c>
       <c r="G22">
-        <v>32.405000000000001</v>
+        <v>32.405</v>
       </c>
       <c r="H22">
         <v>972042.3</v>
@@ -2056,7 +1990,7 @@
         <v>2065</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:12">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -2076,7 +2010,7 @@
         <v>94</v>
       </c>
       <c r="G23">
-        <v>33.957000000000001</v>
+        <v>33.957</v>
       </c>
       <c r="H23">
         <v>1740879.6</v>
@@ -2094,7 +2028,7 @@
         <v>7685</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:12">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -2114,10 +2048,10 @@
         <v>95</v>
       </c>
       <c r="G24">
-        <v>30.234000000000002</v>
+        <v>30.234</v>
       </c>
       <c r="H24">
-        <v>1050944.3999999999</v>
+        <v>1050944.4</v>
       </c>
       <c r="I24" t="s">
         <v>220</v>
@@ -2132,7 +2066,7 @@
         <v>2903</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:12">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -2152,7 +2086,7 @@
         <v>96</v>
       </c>
       <c r="G25">
-        <v>29.388999999999999</v>
+        <v>29.389</v>
       </c>
       <c r="H25">
         <v>838351</v>
@@ -2170,7 +2104,7 @@
         <v>2802</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:12">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -2190,7 +2124,7 @@
         <v>97</v>
       </c>
       <c r="G26">
-        <v>37.551000000000002</v>
+        <v>37.551</v>
       </c>
       <c r="H26">
         <v>24689589.5</v>
@@ -2208,7 +2142,7 @@
         <v>210522</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:12">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -2228,7 +2162,7 @@
         <v>98</v>
       </c>
       <c r="G27">
-        <v>33.027999999999999</v>
+        <v>33.028</v>
       </c>
       <c r="H27">
         <v>958643.5</v>
@@ -2246,7 +2180,7 @@
         <v>8937</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:12">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -2266,7 +2200,7 @@
         <v>99</v>
       </c>
       <c r="G28">
-        <v>32.853999999999999</v>
+        <v>32.854</v>
       </c>
       <c r="H28">
         <v>1184315.3</v>
@@ -2284,7 +2218,7 @@
         <v>3756</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:12">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -2304,7 +2238,7 @@
         <v>100</v>
       </c>
       <c r="G29">
-        <v>35.276000000000003</v>
+        <v>35.276</v>
       </c>
       <c r="H29">
         <v>1036525.5</v>
@@ -2322,7 +2256,7 @@
         <v>5464</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:12">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -2342,10 +2276,10 @@
         <v>101</v>
       </c>
       <c r="G30">
-        <v>31.603000000000002</v>
+        <v>31.603</v>
       </c>
       <c r="H30">
-        <v>82826.600000000006</v>
+        <v>82826.60000000001</v>
       </c>
       <c r="I30" t="s">
         <v>226</v>
@@ -2360,7 +2294,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:12">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -2383,7 +2317,7 @@
         <v>31.134</v>
       </c>
       <c r="H31">
-        <v>2399187.2000000002</v>
+        <v>2399187.2</v>
       </c>
       <c r="I31" t="s">
         <v>227</v>
@@ -2398,7 +2332,7 @@
         <v>16160</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:12">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -2418,10 +2352,10 @@
         <v>103</v>
       </c>
       <c r="G32">
-        <v>41.558999999999997</v>
+        <v>41.559</v>
       </c>
       <c r="H32">
-        <v>80257344.200000003</v>
+        <v>80257344.2</v>
       </c>
       <c r="I32" t="s">
         <v>228</v>
@@ -2436,7 +2370,7 @@
         <v>1473566</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:12">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -2474,7 +2408,7 @@
         <v>5091</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:12">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -2512,7 +2446,7 @@
         <v>4629</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:12">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -2532,7 +2466,7 @@
         <v>106</v>
       </c>
       <c r="G35">
-        <v>32.298999999999999</v>
+        <v>32.299</v>
       </c>
       <c r="H35">
         <v>1025777.2</v>
@@ -2550,7 +2484,7 @@
         <v>6669</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:12">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -2573,7 +2507,7 @@
         <v>52.814</v>
       </c>
       <c r="H36">
-        <v>58936669.299999997</v>
+        <v>58936669.3</v>
       </c>
       <c r="I36" t="s">
         <v>232</v>
@@ -2588,7 +2522,7 @@
         <v>456761</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:12">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -2626,7 +2560,7 @@
         <v>28346</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:12">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -2646,10 +2580,10 @@
         <v>109</v>
       </c>
       <c r="G38">
-        <v>35.293999999999997</v>
+        <v>35.294</v>
       </c>
       <c r="H38">
-        <v>5128666.5999999996</v>
+        <v>5128666.6</v>
       </c>
       <c r="I38" t="s">
         <v>234</v>
@@ -2664,7 +2598,7 @@
         <v>35614</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:12">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -2684,7 +2618,7 @@
         <v>110</v>
       </c>
       <c r="G39">
-        <v>35.905999999999999</v>
+        <v>35.906</v>
       </c>
       <c r="H39">
         <v>3069865.5</v>
@@ -2702,7 +2636,7 @@
         <v>8810</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:12">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -2740,7 +2674,7 @@
         <v>104956</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:12">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -2760,10 +2694,10 @@
         <v>112</v>
       </c>
       <c r="G41">
-        <v>31.818000000000001</v>
+        <v>31.818</v>
       </c>
       <c r="H41">
-        <v>2610294.2000000002</v>
+        <v>2610294.2</v>
       </c>
       <c r="I41" t="s">
         <v>237</v>
@@ -2778,7 +2712,7 @@
         <v>6028</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:12">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -2798,10 +2732,10 @@
         <v>113</v>
       </c>
       <c r="G42">
-        <v>28.172999999999998</v>
+        <v>28.173</v>
       </c>
       <c r="H42">
-        <v>1302227.1000000001</v>
+        <v>1302227.1</v>
       </c>
       <c r="I42" t="s">
         <v>238</v>
@@ -2816,7 +2750,7 @@
         <v>4270</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:12">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -2836,10 +2770,10 @@
         <v>114</v>
       </c>
       <c r="G43">
-        <v>39.755000000000003</v>
+        <v>39.755</v>
       </c>
       <c r="H43">
-        <v>63935238.700000003</v>
+        <v>63935238.7</v>
       </c>
       <c r="I43" t="s">
         <v>239</v>
@@ -2854,7 +2788,7 @@
         <v>1456623</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:12">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -2874,7 +2808,7 @@
         <v>115</v>
       </c>
       <c r="G44">
-        <v>41.646999999999998</v>
+        <v>41.647</v>
       </c>
       <c r="H44">
         <v>4565659.7</v>
@@ -2892,7 +2826,7 @@
         <v>23912</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:12">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -2912,10 +2846,10 @@
         <v>116</v>
       </c>
       <c r="G45">
-        <v>42.697000000000003</v>
+        <v>42.697</v>
       </c>
       <c r="H45">
-        <v>10395197.300000001</v>
+        <v>10395197.3</v>
       </c>
       <c r="I45" t="s">
         <v>241</v>
@@ -2930,7 +2864,7 @@
         <v>97740</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:12">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -2950,7 +2884,7 @@
         <v>117</v>
       </c>
       <c r="G46">
-        <v>30.882000000000001</v>
+        <v>30.882</v>
       </c>
       <c r="H46">
         <v>2075579.4</v>
@@ -2968,7 +2902,7 @@
         <v>8044</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:12">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -2991,7 +2925,7 @@
         <v>46.71</v>
       </c>
       <c r="H47">
-        <v>8346047.4000000004</v>
+        <v>8346047.4</v>
       </c>
       <c r="I47" t="s">
         <v>243</v>
@@ -3006,7 +2940,7 @@
         <v>18055</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:12">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -3026,7 +2960,7 @@
         <v>119</v>
       </c>
       <c r="G48">
-        <v>37.356000000000002</v>
+        <v>37.356</v>
       </c>
       <c r="H48">
         <v>3892732.7</v>
@@ -3044,7 +2978,7 @@
         <v>38095</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:12">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -3064,7 +2998,7 @@
         <v>120</v>
       </c>
       <c r="G49">
-        <v>33.563000000000002</v>
+        <v>33.563</v>
       </c>
       <c r="H49">
         <v>733691.9</v>
@@ -3082,7 +3016,7 @@
         <v>1918</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:12">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -3102,7 +3036,7 @@
         <v>121</v>
       </c>
       <c r="G50">
-        <v>32.113999999999997</v>
+        <v>32.114</v>
       </c>
       <c r="H50">
         <v>377443.2</v>
@@ -3120,7 +3054,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:12">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -3140,7 +3074,7 @@
         <v>122</v>
       </c>
       <c r="G51">
-        <v>31.998000000000001</v>
+        <v>31.998</v>
       </c>
       <c r="H51">
         <v>693479.4</v>
@@ -3158,7 +3092,7 @@
         <v>3291</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:12">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -3196,7 +3130,7 @@
         <v>5739</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:12">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -3219,7 +3153,7 @@
         <v>48.177</v>
       </c>
       <c r="H53">
-        <v>55140618.600000001</v>
+        <v>55140618.6</v>
       </c>
       <c r="I53" t="s">
         <v>249</v>
@@ -3234,7 +3168,7 @@
         <v>319503</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:12">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -3254,7 +3188,7 @@
         <v>125</v>
       </c>
       <c r="G54">
-        <v>35.798000000000002</v>
+        <v>35.798</v>
       </c>
       <c r="H54">
         <v>1794190.4</v>
@@ -3272,7 +3206,7 @@
         <v>16343</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:12">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -3292,7 +3226,7 @@
         <v>126</v>
       </c>
       <c r="G55">
-        <v>35.192999999999998</v>
+        <v>35.193</v>
       </c>
       <c r="H55">
         <v>1171454.7</v>
@@ -3310,7 +3244,7 @@
         <v>2045</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:12">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -3330,7 +3264,7 @@
         <v>127</v>
       </c>
       <c r="G56">
-        <v>29.774000000000001</v>
+        <v>29.774</v>
       </c>
       <c r="H56">
         <v>2701530.3</v>
@@ -3348,7 +3282,7 @@
         <v>20869</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:12">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -3371,7 +3305,7 @@
         <v>36.244</v>
       </c>
       <c r="H57">
-        <v>4810770.9000000004</v>
+        <v>4810770.9</v>
       </c>
       <c r="I57" t="s">
         <v>253</v>
@@ -3386,7 +3320,7 @@
         <v>32308</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:12">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -3406,7 +3340,7 @@
         <v>129</v>
       </c>
       <c r="G58">
-        <v>38.118000000000002</v>
+        <v>38.118</v>
       </c>
       <c r="H58">
         <v>1827294.9</v>
@@ -3424,7 +3358,7 @@
         <v>2892</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:12">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -3444,10 +3378,10 @@
         <v>130</v>
       </c>
       <c r="G59">
-        <v>34.706000000000003</v>
+        <v>34.706</v>
       </c>
       <c r="H59">
-        <v>1285477.3999999999</v>
+        <v>1285477.4</v>
       </c>
       <c r="I59" t="s">
         <v>255</v>
@@ -3462,7 +3396,7 @@
         <v>4531</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:12">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -3482,10 +3416,10 @@
         <v>131</v>
       </c>
       <c r="G60">
-        <v>34.460999999999999</v>
+        <v>34.461</v>
       </c>
       <c r="H60">
-        <v>2153154.2000000002</v>
+        <v>2153154.2</v>
       </c>
       <c r="I60" t="s">
         <v>256</v>
@@ -3500,7 +3434,7 @@
         <v>7504</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:12">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -3520,10 +3454,10 @@
         <v>132</v>
       </c>
       <c r="G61">
-        <v>50.561999999999998</v>
+        <v>50.562</v>
       </c>
       <c r="H61">
-        <v>46222976.200000003</v>
+        <v>46222976.2</v>
       </c>
       <c r="I61" t="s">
         <v>257</v>
@@ -3538,7 +3472,7 @@
         <v>370351</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:12">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -3558,7 +3492,7 @@
         <v>133</v>
       </c>
       <c r="G62">
-        <v>35.082000000000001</v>
+        <v>35.082</v>
       </c>
       <c r="H62">
         <v>893158.6</v>
@@ -3576,7 +3510,7 @@
         <v>3548</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:12">
       <c r="A63" s="1">
         <v>61</v>
       </c>

</xml_diff>